<commit_message>
More OSD updates. New icons. Tidy up slider (still no timeshift info yet)
</commit_message>
<xml_diff>
--- a/MousetuaryTODO.xlsx
+++ b/MousetuaryTODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>Mousetuary TODO list</t>
   </si>
@@ -34,9 +34,6 @@
     <t>Done</t>
   </si>
   <si>
-    <t>Need better handling of maximise from Win titlebar. Bug reported.</t>
-  </si>
-  <si>
     <t>Back and Home to topbar.</t>
   </si>
   <si>
@@ -91,7 +88,34 @@
     <t>Channels and Guide seem redundant.</t>
   </si>
   <si>
-    <t>Can we just have the Guide and get rid of Channels?</t>
+    <t>Smaller and less shouty text in general.</t>
+  </si>
+  <si>
+    <t>It disappears as soon as the mouse is moved, so there's no point to it.</t>
+  </si>
+  <si>
+    <t>Need better handling of maximise from Win titlebar. Bug reported. Once fixed, these buttons can be hidden when windowed.</t>
+  </si>
+  <si>
+    <t>OSD slider can report timeshift buffer extent</t>
+  </si>
+  <si>
+    <t>Like WMC does. Awaiting a PVR backend that reports this information (NextPVR doesn't)</t>
+  </si>
+  <si>
+    <t>Get rid of fwd/back buttons from OSD slider nib</t>
+  </si>
+  <si>
+    <t>VideoOSDHelpTextVar for new buttons (variables.xml)</t>
+  </si>
+  <si>
+    <t>Can we just have the Guide and get rid of Channels? Or merge their functions somehow?</t>
+  </si>
+  <si>
+    <t>Get rid of misleading message for slider</t>
+  </si>
+  <si>
+    <t>Display left-side ones on left, if possible.</t>
   </si>
 </sst>
 </file>
@@ -135,10 +159,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,158 +475,200 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.5546875" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="38.5546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" customWidth="1"/>
+    <col min="3" max="3" width="59.33203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
+      <c r="A2" s="2"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
+      <c r="A4" s="2"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="C24" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Disable side menu (options menu and left side mouse action) as it is non-functional (disappears as soon as the mouse is moved)
</commit_message>
<xml_diff>
--- a/MousetuaryTODO.xlsx
+++ b/MousetuaryTODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>Mousetuary TODO list</t>
   </si>
@@ -116,6 +116,12 @@
   </si>
   <si>
     <t>Display left-side ones on left, if possible.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guide should roll up and down with the mouse wheel, not left to right. </t>
+  </si>
+  <si>
+    <t>Can do in a keymap, but not sure how in a skin. Requested.</t>
   </si>
 </sst>
 </file>
@@ -159,9 +165,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -170,6 +175,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -475,199 +486,210 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.5546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="8.5546875" customWidth="1"/>
-    <col min="3" max="3" width="59.33203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="38.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="59.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2"/>
+      <c r="A2" s="1"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="2"/>
+      <c r="A4" s="1"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="B6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="B9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
+      <c r="A11" s="3"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="B13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="B15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
+      <c r="A21" s="3"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+    <row r="25" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add vertical scrollbars to widget lists off the home menu, at the suggestion of leon_tamp. Change version to 1.0.1 so I can keep track of, and reference, changes.
</commit_message>
<xml_diff>
--- a/MousetuaryTODO.xlsx
+++ b/MousetuaryTODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
   <si>
     <t>Mousetuary TODO list</t>
   </si>
@@ -109,19 +109,64 @@
     <t>VideoOSDHelpTextVar for new buttons (variables.xml)</t>
   </si>
   <si>
-    <t>Can we just have the Guide and get rid of Channels? Or merge their functions somehow?</t>
-  </si>
-  <si>
     <t>Get rid of misleading message for slider</t>
   </si>
   <si>
-    <t>Display left-side ones on left, if possible.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Guide should roll up and down with the mouse wheel, not left to right. </t>
   </si>
   <si>
     <t>Can do in a keymap, but not sure how in a skin. Requested.</t>
+  </si>
+  <si>
+    <t>Guide needs up/down/left/right buttons that appear with a mouse hover, like WMC</t>
+  </si>
+  <si>
+    <t>Guide rows need to be a little bigger, also guide font</t>
+  </si>
+  <si>
+    <t>Autoscroll might also be OK (but not so aggressive as the My Addons list!)</t>
+  </si>
+  <si>
+    <t>Guide and Channels from OSD need the Back button at top left.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display left-side ones on left, if possible. </t>
+  </si>
+  <si>
+    <t>Can we merge these and just show the real Guide?</t>
+  </si>
+  <si>
+    <t>Low priority</t>
+  </si>
+  <si>
+    <t>Needs localize</t>
+  </si>
+  <si>
+    <t>Scroll bars in widget lists</t>
+  </si>
+  <si>
+    <t>Gives a standard way of scrolling them, since autoscroll is not working consistently. The mouse wheel can be used in the scroll bar (while in the widget rows, it scrolls them horizontally)</t>
+  </si>
+  <si>
+    <t>Make Guide come first in widget list</t>
+  </si>
+  <si>
+    <t>Pending decision on the above</t>
+  </si>
+  <si>
+    <t>Can we just have the Guide and get rid of Channels? Or merge their functions somehow? Use full guide from OSD?</t>
+  </si>
+  <si>
+    <t>Fix over-aggressive autoscroll in Addons/MyAddons list</t>
+  </si>
+  <si>
+    <t>It's awful! It should either autoscroll properly, or have a scroll bar.</t>
+  </si>
+  <si>
+    <t>Initiator</t>
+  </si>
+  <si>
+    <t>leon_tamp</t>
   </si>
 </sst>
 </file>
@@ -165,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -175,12 +220,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -486,215 +525,282 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="38.5546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.5546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="59.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="4"/>
+      <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="4"/>
+      <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="B10" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="C10" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+    <row r="11" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="B15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+      <c r="B16" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="B17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="B21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="3"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+    <row r="30" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C30" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="82" fitToWidth="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix todo list to reflect last commit...
</commit_message>
<xml_diff>
--- a/MousetuaryTODO.xlsx
+++ b/MousetuaryTODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
   <si>
     <t>Mousetuary TODO list</t>
   </si>
@@ -127,15 +127,9 @@
     <t>Autoscroll might also be OK (but not so aggressive as the My Addons list!)</t>
   </si>
   <si>
-    <t>Guide and Channels from OSD need the Back button at top left.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Display left-side ones on left, if possible. </t>
   </si>
   <si>
-    <t>Can we merge these and just show the real Guide?</t>
-  </si>
-  <si>
     <t>Low priority</t>
   </si>
   <si>
@@ -154,9 +148,6 @@
     <t>Pending decision on the above</t>
   </si>
   <si>
-    <t>Can we just have the Guide and get rid of Channels? Or merge their functions somehow? Use full guide from OSD?</t>
-  </si>
-  <si>
     <t>Fix over-aggressive autoscroll in Addons/MyAddons list</t>
   </si>
   <si>
@@ -167,6 +158,12 @@
   </si>
   <si>
     <t>leon_tamp</t>
+  </si>
+  <si>
+    <t>Use full guide rather than the abbreviated OSD guide. Remove OSD channel button.</t>
+  </si>
+  <si>
+    <t>Can we just have the Guide and get rid of Channels? For the moment, just make guide the first widget in the line.</t>
   </si>
 </sst>
 </file>
@@ -530,8 +527,8 @@
   </sheetPr>
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -565,7 +562,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -624,7 +621,7 @@
         <v>21</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>22</v>
@@ -632,24 +629,24 @@
     </row>
     <row r="11" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -716,10 +713,10 @@
         <v>30</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -732,10 +729,10 @@
     </row>
     <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>39</v>
+        <v>48</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -759,18 +756,18 @@
         <v>23</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Reinstate side menu. Control by a window property (in the manner of Aeon Nox 5) rather than relying on focus. Dismiss with a back button.
</commit_message>
<xml_diff>
--- a/MousetuaryTODO.xlsx
+++ b/MousetuaryTODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
   <si>
     <t>Mousetuary TODO list</t>
   </si>
@@ -61,24 +61,15 @@
     <t>OSD transparent background colour nicer</t>
   </si>
   <si>
-    <t>Home Screen and Menus</t>
-  </si>
-  <si>
     <t>Video OSD</t>
   </si>
   <si>
-    <t>Live TV menu</t>
-  </si>
-  <si>
     <t>Right-click option to delete recent channels from list</t>
   </si>
   <si>
     <t>More right-clicky stuff in general would be nice.</t>
   </si>
   <si>
-    <t>Other menus</t>
-  </si>
-  <si>
     <t>Sensible defaults</t>
   </si>
   <si>
@@ -91,9 +82,6 @@
     <t>Smaller and less shouty text in general.</t>
   </si>
   <si>
-    <t>It disappears as soon as the mouse is moved, so there's no point to it.</t>
-  </si>
-  <si>
     <t>Need better handling of maximise from Win titlebar. Bug reported. Once fixed, these buttons can be hidden when windowed.</t>
   </si>
   <si>
@@ -164,6 +152,21 @@
   </si>
   <si>
     <t>Can we just have the Guide and get rid of Channels? For the moment, just make guide the first widget in the line.</t>
+  </si>
+  <si>
+    <t>TV Guide</t>
+  </si>
+  <si>
+    <t>Live TV widget list</t>
+  </si>
+  <si>
+    <t>Home Screen and widget lists</t>
+  </si>
+  <si>
+    <t>Reinstated</t>
+  </si>
+  <si>
+    <t>Fixed losing focus by using a window property, like Aeon Nox 5 does. Dismiss by a back button.</t>
   </si>
 </sst>
 </file>
@@ -525,16 +528,16 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="38.5546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="59.33203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="15.5546875" customWidth="1"/>
   </cols>
@@ -562,7 +565,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -572,7 +575,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -583,7 +586,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -602,51 +605,51 @@
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -654,7 +657,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -694,7 +697,7 @@
     </row>
     <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>5</v>
@@ -702,26 +705,26 @@
     </row>
     <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>5</v>
@@ -729,7 +732,7 @@
     </row>
     <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>5</v>
@@ -740,61 +743,64 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>20</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add optional keymap and script to map some media keys to WMC behaviour (wheel scrolling in guide, next/prev track for skipping, and ctrl-g for guide from live TV)
</commit_message>
<xml_diff>
--- a/MousetuaryTODO.xlsx
+++ b/MousetuaryTODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
   <si>
     <t>Mousetuary TODO list</t>
   </si>
@@ -103,9 +103,6 @@
     <t xml:space="preserve">Guide should roll up and down with the mouse wheel, not left to right. </t>
   </si>
   <si>
-    <t>Can do in a keymap, but not sure how in a skin. Requested.</t>
-  </si>
-  <si>
     <t>Guide needs up/down/left/right buttons that appear with a mouse hover, like WMC</t>
   </si>
   <si>
@@ -167,6 +164,12 @@
   </si>
   <si>
     <t>Fixed losing focus by using a window property, like Aeon Nox 5 does. Dismiss by a back button.</t>
+  </si>
+  <si>
+    <t>Done using a keymap. Ctrl-g for guide with support of a script.</t>
+  </si>
+  <si>
+    <t>Done-ish</t>
   </si>
 </sst>
 </file>
@@ -530,8 +533,8 @@
   </sheetPr>
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -565,7 +568,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -575,7 +578,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -613,10 +616,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -624,7 +627,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>19</v>
@@ -632,24 +635,24 @@
     </row>
     <row r="11" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="D11" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -716,10 +719,10 @@
         <v>26</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -732,7 +735,7 @@
     </row>
     <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>5</v>
@@ -743,7 +746,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -758,45 +761,51 @@
       <c r="A27" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="B27" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="C27" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="B31" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="C31" s="2" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Set dark blue tint on OSD fade background (just because it looks nice like WMC) and control it with a color in colors/defaults.xml. Also make start on help messages for new video OSD buttons (split into left and right groups)
</commit_message>
<xml_diff>
--- a/MousetuaryTODO.xlsx
+++ b/MousetuaryTODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
   <si>
     <t>Mousetuary TODO list</t>
   </si>
@@ -25,9 +25,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Comments</t>
-  </si>
-  <si>
     <t>Sysmenu: minimise, window, exit</t>
   </si>
   <si>
@@ -109,9 +106,6 @@
     <t>Guide rows need to be a little bigger, also guide font</t>
   </si>
   <si>
-    <t>Autoscroll might also be OK (but not so aggressive as the My Addons list!)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Display left-side ones on left, if possible. </t>
   </si>
   <si>
@@ -163,13 +157,28 @@
     <t>Reinstated</t>
   </si>
   <si>
-    <t>Fixed losing focus by using a window property, like Aeon Nox 5 does. Dismiss by a back button.</t>
-  </si>
-  <si>
-    <t>Done using a keymap. Ctrl-g for guide with support of a script.</t>
-  </si>
-  <si>
     <t>Done-ish</t>
+  </si>
+  <si>
+    <t>Comments/Issues</t>
+  </si>
+  <si>
+    <t>Fixed losing focus by using a window property, like Aeon Nox 5 does. Options button up in top bar. Dismiss by a back button.</t>
+  </si>
+  <si>
+    <t>Make it blue like WMC.</t>
+  </si>
+  <si>
+    <t>Autoscroll might also be OK (but not so aggressive as the My Addons list!). Problem is, no button seems to be able to control the EPGGrid.</t>
+  </si>
+  <si>
+    <t>Parameterise the EPG row size and font size (maybe even put in settings)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Done using a keymap. </t>
+  </si>
+  <si>
+    <t>Ctrl-g for guide with support of a script (goes with optional keymap)</t>
   </si>
 </sst>
 </file>
@@ -533,8 +542,8 @@
   </sheetPr>
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -565,10 +574,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -578,45 +587,45 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>49</v>
@@ -624,35 +633,35 @@
     </row>
     <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -660,85 +669,94 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -746,69 +764,72 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C33" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add U/D/L/R buttons to guide to scroll the EPG. (a page at a time up/down, and a program slot at a time left/right)
</commit_message>
<xml_diff>
--- a/MousetuaryTODO.xlsx
+++ b/MousetuaryTODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
   <si>
     <t>Mousetuary TODO list</t>
   </si>
@@ -167,12 +167,6 @@
   </si>
   <si>
     <t>Make it blue like WMC.</t>
-  </si>
-  <si>
-    <t>Autoscroll might also be OK (but not so aggressive as the My Addons list!). Problem is, no button seems to be able to control the EPGGrid.</t>
-  </si>
-  <si>
-    <t>Parameterise the EPG row size and font size (maybe even put in settings)</t>
   </si>
   <si>
     <t xml:space="preserve">Done using a keymap. </t>
@@ -543,7 +537,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -756,7 +750,7 @@
         <v>4</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -810,26 +804,26 @@
         <v>4</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B32" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B33" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bring Music OSD into line with video OSD. (buttons, sizes, slider)
</commit_message>
<xml_diff>
--- a/MousetuaryTODO.xlsx
+++ b/MousetuaryTODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="54">
   <si>
     <t>Mousetuary TODO list</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Right-click option to delete recent channels from list</t>
   </si>
   <si>
-    <t>More right-clicky stuff in general would be nice.</t>
-  </si>
-  <si>
     <t>Sensible defaults</t>
   </si>
   <si>
@@ -173,6 +170,12 @@
   </si>
   <si>
     <t>Ctrl-g for guide with support of a script (goes with optional keymap)</t>
+  </si>
+  <si>
+    <t>Not skinnable</t>
+  </si>
+  <si>
+    <t>There is very limited scope for skins to do this (existing context menus ca be added to, but new ones can't be created)</t>
   </si>
 </sst>
 </file>
@@ -536,8 +539,8 @@
   </sheetPr>
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -568,10 +571,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -581,7 +584,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -592,7 +595,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -611,7 +614,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -619,43 +622,43 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="D11" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -704,12 +707,12 @@
         <v>4</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>4</v>
@@ -717,26 +720,26 @@
     </row>
     <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>4</v>
@@ -744,13 +747,13 @@
     </row>
     <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -758,58 +761,61 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="B26" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="C26" s="2" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>4</v>
@@ -817,7 +823,7 @@
     </row>
     <row r="33" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Tidy up dead test code in OSD. Make sure skip buttons are hidden when play/pause is hidden (if seeking not enabled)
</commit_message>
<xml_diff>
--- a/MousetuaryTODO.xlsx
+++ b/MousetuaryTODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="54">
   <si>
     <t>Mousetuary TODO list</t>
   </si>
@@ -79,12 +79,6 @@
     <t>Need better handling of maximise from Win titlebar. Bug reported. Once fixed, these buttons can be hidden when windowed.</t>
   </si>
   <si>
-    <t>OSD slider can report timeshift buffer extent</t>
-  </si>
-  <si>
-    <t>Like WMC does. Awaiting a PVR backend that reports this information (NextPVR doesn't)</t>
-  </si>
-  <si>
     <t>Get rid of fwd/back buttons from OSD slider nib</t>
   </si>
   <si>
@@ -176,6 +170,12 @@
   </si>
   <si>
     <t>There is very limited scope for skins to do this (existing context menus ca be added to, but new ones can't be created)</t>
+  </si>
+  <si>
+    <t>OSD slider can report timeshift buffer extent to scale, like WMC does</t>
+  </si>
+  <si>
+    <t>Need to display a calculated progress based on several infotags. Can't do this in the skinning engine.</t>
   </si>
 </sst>
 </file>
@@ -539,8 +539,8 @@
   </sheetPr>
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -571,10 +571,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -584,7 +584,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -622,10 +622,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -633,7 +633,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>17</v>
@@ -641,24 +641,24 @@
     </row>
     <row r="11" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -707,12 +707,12 @@
         <v>4</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>4</v>
@@ -720,26 +720,29 @@
     </row>
     <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>21</v>
+        <v>52</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>4</v>
@@ -747,13 +750,13 @@
     </row>
     <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -761,7 +764,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -769,10 +772,10 @@
         <v>15</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -780,42 +783,42 @@
         <v>18</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>4</v>
@@ -823,7 +826,7 @@
     </row>
     <row r="33" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Update changelog and close off 1.0.1.
</commit_message>
<xml_diff>
--- a/MousetuaryTODO.xlsx
+++ b/MousetuaryTODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="56">
   <si>
     <t>Mousetuary TODO list</t>
   </si>
@@ -103,9 +103,6 @@
     <t>Low priority</t>
   </si>
   <si>
-    <t>Needs localize</t>
-  </si>
-  <si>
     <t>Scroll bars in widget lists</t>
   </si>
   <si>
@@ -124,12 +121,6 @@
     <t>It's awful! It should either autoscroll properly, or have a scroll bar.</t>
   </si>
   <si>
-    <t>Initiator</t>
-  </si>
-  <si>
-    <t>leon_tamp</t>
-  </si>
-  <si>
     <t>Use full guide rather than the abbreviated OSD guide. Remove OSD channel button.</t>
   </si>
   <si>
@@ -157,9 +148,6 @@
     <t>Fixed losing focus by using a window property, like Aeon Nox 5 does. Options button up in top bar. Dismiss by a back button.</t>
   </si>
   <si>
-    <t>Make it blue like WMC.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Done using a keymap. </t>
   </si>
   <si>
@@ -176,6 +164,24 @@
   </si>
   <si>
     <t>Need to display a calculated progress based on several infotags. Can't do this in the skinning engine.</t>
+  </si>
+  <si>
+    <t>Make it blue like WMC. Also make a semitransparent blue background for the guide when live video is in progress.</t>
+  </si>
+  <si>
+    <t>Started</t>
+  </si>
+  <si>
+    <t>Not done</t>
+  </si>
+  <si>
+    <t>1.0.1</t>
+  </si>
+  <si>
+    <t>1.0.2</t>
+  </si>
+  <si>
+    <t>Incomplete:</t>
   </si>
 </sst>
 </file>
@@ -537,10 +543,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,7 +565,9 @@
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
@@ -571,11 +579,9 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>36</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
@@ -584,7 +590,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -622,10 +628,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -641,199 +647,207 @@
     </row>
     <row r="11" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C16" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>52</v>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="B35" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="2" t="s">
+    <row r="36" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="3"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Provide a skin setting to control genre coloring in the EPG. (I dislike it, but some may disagree)
</commit_message>
<xml_diff>
--- a/MousetuaryTODO.xlsx
+++ b/MousetuaryTODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
   <si>
     <t>Mousetuary TODO list</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t>Incomplete:</t>
+  </si>
+  <si>
+    <t>Provide setting to control genre coloring</t>
   </si>
 </sst>
 </file>
@@ -543,10 +546,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -800,52 +803,68 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
+    <row r="38" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
+    <row r="39" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
+    <row r="40" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
+    <row r="41" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add python script to implement progress bar for timeshift on scale of OSD slider. Tidy up timeshift display in seek bar.
</commit_message>
<xml_diff>
--- a/MousetuaryTODO.xlsx
+++ b/MousetuaryTODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
   <si>
     <t>Mousetuary TODO list</t>
   </si>
@@ -157,15 +157,9 @@
     <t>Not skinnable</t>
   </si>
   <si>
-    <t>There is very limited scope for skins to do this (existing context menus ca be added to, but new ones can't be created)</t>
-  </si>
-  <si>
     <t>OSD slider can report timeshift buffer extent to scale, like WMC does</t>
   </si>
   <si>
-    <t>Need to display a calculated progress based on several infotags. Can't do this in the skinning engine.</t>
-  </si>
-  <si>
     <t>Make it blue like WMC. Also make a semitransparent blue background for the guide when live video is in progress.</t>
   </si>
   <si>
@@ -185,6 +179,15 @@
   </si>
   <si>
     <t>Provide setting to control genre coloring</t>
+  </si>
+  <si>
+    <t>Partially done</t>
+  </si>
+  <si>
+    <t>Done with Python script. Still awaiting bug fix for Player.Progress (bug tracker #17469)</t>
+  </si>
+  <si>
+    <t>There is very limited scope for skins to do this (existing context menus can be added to, but new ones can't be created)</t>
   </si>
 </sst>
 </file>
@@ -548,8 +551,8 @@
   </sheetPr>
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -569,7 +572,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -706,7 +709,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -800,7 +803,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -810,7 +813,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>4</v>
@@ -821,7 +824,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -829,7 +832,7 @@
         <v>33</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>34</v>
@@ -840,7 +843,7 @@
         <v>22</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>27</v>
@@ -854,18 +857,18 @@
         <v>46</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some changes to improve touch support on small screens (it's not just for mice!)
</commit_message>
<xml_diff>
--- a/MousetuaryTODO.xlsx
+++ b/MousetuaryTODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="60">
   <si>
     <t>Mousetuary TODO list</t>
   </si>
@@ -188,6 +188,12 @@
   </si>
   <si>
     <t>There is very limited scope for skins to do this (existing context menus can be added to, but new ones can't be created)</t>
+  </si>
+  <si>
+    <t>Some changes to improve touch support on small screens (it's not just for mice!)</t>
+  </si>
+  <si>
+    <t>Now you don't have to use Estouchy.</t>
   </si>
 </sst>
 </file>
@@ -549,10 +555,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -806,68 +812,79 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+    <row r="33" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="1"/>
+      <c r="B36" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="1"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="3" t="s">
+    <row r="42" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Split video OSD slider into two, one to display PVR.Progress, and the other to actually do the seek. This was needed because a seeking slider cannot display anything other than Player.Progress, which does not reflect the timeshifted position. Also add help strings for new buttons in the OSD.
</commit_message>
<xml_diff>
--- a/MousetuaryTODO.xlsx
+++ b/MousetuaryTODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
   <si>
     <t>Mousetuary TODO list</t>
   </si>
@@ -82,9 +82,6 @@
     <t>Get rid of fwd/back buttons from OSD slider nib</t>
   </si>
   <si>
-    <t>VideoOSDHelpTextVar for new buttons (variables.xml)</t>
-  </si>
-  <si>
     <t>Get rid of misleading message for slider</t>
   </si>
   <si>
@@ -97,9 +94,6 @@
     <t>Guide rows need to be a little bigger, also guide font</t>
   </si>
   <si>
-    <t xml:space="preserve">Display left-side ones on left, if possible. </t>
-  </si>
-  <si>
     <t>Low priority</t>
   </si>
   <si>
@@ -163,9 +157,6 @@
     <t>Make it blue like WMC. Also make a semitransparent blue background for the guide when live video is in progress.</t>
   </si>
   <si>
-    <t>Started</t>
-  </si>
-  <si>
     <t>Not done</t>
   </si>
   <si>
@@ -181,12 +172,6 @@
     <t>Provide setting to control genre coloring</t>
   </si>
   <si>
-    <t>Partially done</t>
-  </si>
-  <si>
-    <t>Done with Python script. Still awaiting bug fix for Player.Progress (bug tracker #17469)</t>
-  </si>
-  <si>
     <t>There is very limited scope for skins to do this (existing context menus can be added to, but new ones can't be created)</t>
   </si>
   <si>
@@ -194,6 +179,21 @@
   </si>
   <si>
     <t>Now you don't have to use Estouchy.</t>
+  </si>
+  <si>
+    <t>1.0.3</t>
+  </si>
+  <si>
+    <t>Split slider into two, one to seek and the other to show PVR.Progress</t>
+  </si>
+  <si>
+    <t>Action "seek" will only display Player.Progress, which does not show the timeshifted position.</t>
+  </si>
+  <si>
+    <t>Done with Python script. Bug reported for Player.Progress (bug tracker #17469) but 1.0.3 has a fix for this.</t>
+  </si>
+  <si>
+    <t>Add VideoOSDHelpTextVar strings for new buttons (variables.xml)</t>
   </si>
 </sst>
 </file>
@@ -555,10 +555,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -578,7 +578,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -591,7 +591,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -602,7 +602,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -640,10 +640,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -651,7 +651,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>17</v>
@@ -659,13 +659,13 @@
     </row>
     <row r="11" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D11" s="2"/>
     </row>
@@ -715,7 +715,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -728,7 +728,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>4</v>
@@ -736,13 +736,13 @@
     </row>
     <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -750,7 +750,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -758,42 +758,42 @@
         <v>18</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>4</v>
@@ -801,7 +801,7 @@
     </row>
     <row r="30" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>4</v>
@@ -809,83 +809,96 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="1"/>
+      <c r="A37" s="3"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
-        <v>33</v>
+      <c r="A39" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="3"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
+    </row>
+    <row r="44" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>56</v>
+      <c r="B45" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>